<commit_message>
fix: try to fix Dockerfile #2
</commit_message>
<xml_diff>
--- a/model_3/dataset_workout.xlsx
+++ b/model_3/dataset_workout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@KULIAH\SEMESTER 7\BANGKIT 2023 BATCH 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\RoadtoFit-ML\model_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F611C3E-E42A-427E-A14E-93287BE62782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDD51F1-CCA4-4630-9499-621B52AC31C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5118DCE0-E9E8-4C82-B416-7D665D3D04FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5118DCE0-E9E8-4C82-B416-7D665D3D04FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="170">
   <si>
     <t>kal/jam</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>lacrosse (permainan bola dengan tongkat)</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -914,18 +917,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6034F0EE-07D5-4E91-9989-1AE65625C2B3}">
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E161" sqref="E161"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -935,8 +938,11 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -946,8 +952,11 @@
       <c r="C2">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -957,8 +966,11 @@
       <c r="C3">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -968,8 +980,11 @@
       <c r="C4">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -979,8 +994,11 @@
       <c r="C5">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -990,8 +1008,11 @@
       <c r="C6">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1001,8 +1022,11 @@
       <c r="C7">
         <v>220</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1012,8 +1036,11 @@
       <c r="C8">
         <v>147</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1023,8 +1050,11 @@
       <c r="C9">
         <v>147</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1034,8 +1064,11 @@
       <c r="C10">
         <v>147</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1045,8 +1078,11 @@
       <c r="C11">
         <v>147</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1056,8 +1092,11 @@
       <c r="C12">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1067,8 +1106,11 @@
       <c r="C13">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1078,8 +1120,11 @@
       <c r="C14">
         <v>147</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1089,8 +1134,11 @@
       <c r="C15">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1100,8 +1148,11 @@
       <c r="C16">
         <v>147</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1111,8 +1162,11 @@
       <c r="C17">
         <v>147</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1122,8 +1176,11 @@
       <c r="C18">
         <v>147</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1133,8 +1190,11 @@
       <c r="C19">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1144,8 +1204,11 @@
       <c r="C20">
         <v>147</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1155,8 +1218,11 @@
       <c r="C21">
         <v>147</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1166,8 +1232,11 @@
       <c r="C22">
         <v>147</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1177,8 +1246,11 @@
       <c r="C23">
         <v>147</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1188,8 +1260,11 @@
       <c r="C24">
         <v>220</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -1199,8 +1274,11 @@
       <c r="C25">
         <v>220</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1210,8 +1288,11 @@
       <c r="C26">
         <v>220</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1221,8 +1302,11 @@
       <c r="C27">
         <v>220</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1232,8 +1316,11 @@
       <c r="C28">
         <v>220</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1243,8 +1330,11 @@
       <c r="C29">
         <v>220</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1254,8 +1344,11 @@
       <c r="C30">
         <v>220</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1265,8 +1358,11 @@
       <c r="C31">
         <v>220</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1276,8 +1372,11 @@
       <c r="C32">
         <v>220</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1287,8 +1386,11 @@
       <c r="C33">
         <v>228</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -1298,8 +1400,11 @@
       <c r="C34">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -1309,8 +1414,11 @@
       <c r="C35">
         <v>257</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1320,8 +1428,11 @@
       <c r="C36">
         <v>279</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -1331,8 +1442,11 @@
       <c r="C37">
         <v>294</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -1342,8 +1456,11 @@
       <c r="C38">
         <v>294</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1353,8 +1470,11 @@
       <c r="C39">
         <v>294</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1364,8 +1484,11 @@
       <c r="C40">
         <v>294</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -1375,8 +1498,11 @@
       <c r="C41">
         <v>294</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -1386,8 +1512,11 @@
       <c r="C42">
         <v>294</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -1397,8 +1526,11 @@
       <c r="C43">
         <v>294</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -1408,8 +1540,11 @@
       <c r="C44">
         <v>294</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -1419,8 +1554,11 @@
       <c r="C45">
         <v>294</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -1430,8 +1568,11 @@
       <c r="C46">
         <v>294</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1441,8 +1582,11 @@
       <c r="C47">
         <v>294</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1452,8 +1596,11 @@
       <c r="C48">
         <v>294</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -1463,8 +1610,11 @@
       <c r="C49">
         <v>294</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
@@ -1474,8 +1624,11 @@
       <c r="C50">
         <v>294</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -1485,8 +1638,11 @@
       <c r="C51">
         <v>368</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
@@ -1496,8 +1652,11 @@
       <c r="C52">
         <v>368</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -1507,8 +1666,11 @@
       <c r="C53">
         <v>368</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -1518,8 +1680,11 @@
       <c r="C54">
         <v>368</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
@@ -1529,8 +1694,11 @@
       <c r="C55">
         <v>368</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -1540,8 +1708,11 @@
       <c r="C56">
         <v>368</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
@@ -1551,8 +1722,11 @@
       <c r="C57">
         <v>368</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
@@ -1562,8 +1736,11 @@
       <c r="C58">
         <v>368</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
@@ -1573,8 +1750,11 @@
       <c r="C59">
         <v>368</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
@@ -1584,8 +1764,11 @@
       <c r="C60">
         <v>368</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -1595,8 +1778,11 @@
       <c r="C61">
         <v>368</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
@@ -1606,8 +1792,11 @@
       <c r="C62">
         <v>368</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
@@ -1617,8 +1806,11 @@
       <c r="C63">
         <v>368</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -1628,8 +1820,11 @@
       <c r="C64">
         <v>441</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
@@ -1639,8 +1834,11 @@
       <c r="C65">
         <v>441</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
@@ -1650,8 +1848,11 @@
       <c r="C66">
         <v>441</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
@@ -1661,8 +1862,11 @@
       <c r="C67">
         <v>441</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -1672,8 +1876,11 @@
       <c r="C68">
         <v>441</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>71</v>
       </c>
@@ -1683,8 +1890,11 @@
       <c r="C69">
         <v>441</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
@@ -1694,8 +1904,11 @@
       <c r="C70">
         <v>441</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
@@ -1705,8 +1918,11 @@
       <c r="C71">
         <v>441</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
@@ -1716,8 +1932,11 @@
       <c r="C72">
         <v>441</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
@@ -1727,8 +1946,11 @@
       <c r="C73">
         <v>441</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>76</v>
       </c>
@@ -1738,8 +1960,11 @@
       <c r="C74">
         <v>441</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
@@ -1749,8 +1974,11 @@
       <c r="C75">
         <v>441</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -1760,8 +1988,11 @@
       <c r="C76">
         <v>441</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
@@ -1771,8 +2002,11 @@
       <c r="C77">
         <v>441</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
@@ -1782,8 +2016,11 @@
       <c r="C78">
         <v>441</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>81</v>
       </c>
@@ -1793,8 +2030,11 @@
       <c r="C79">
         <v>441</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -1804,8 +2044,11 @@
       <c r="C80">
         <v>441</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -1815,8 +2058,11 @@
       <c r="C81">
         <v>514</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
@@ -1826,8 +2072,11 @@
       <c r="C82">
         <v>514</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -1837,8 +2086,11 @@
       <c r="C83">
         <v>514</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>87</v>
       </c>
@@ -1848,8 +2100,11 @@
       <c r="C84">
         <v>514</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>88</v>
       </c>
@@ -1859,8 +2114,11 @@
       <c r="C85">
         <v>514</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>89</v>
       </c>
@@ -1870,8 +2128,11 @@
       <c r="C86">
         <v>514</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>90</v>
       </c>
@@ -1881,8 +2142,11 @@
       <c r="C87">
         <v>514</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
@@ -1892,8 +2156,11 @@
       <c r="C88">
         <v>514</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>92</v>
       </c>
@@ -1903,8 +2170,11 @@
       <c r="C89">
         <v>514</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>93</v>
       </c>
@@ -1914,8 +2184,11 @@
       <c r="C90">
         <v>514</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
@@ -1925,8 +2198,11 @@
       <c r="C91">
         <v>514</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -1936,8 +2212,11 @@
       <c r="C92">
         <v>514</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -1947,8 +2226,11 @@
       <c r="C93">
         <v>514</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -1958,8 +2240,11 @@
       <c r="C94">
         <v>514</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -1969,8 +2254,11 @@
       <c r="C95">
         <v>514</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
@@ -1980,8 +2268,11 @@
       <c r="C96">
         <v>514</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -1991,8 +2282,11 @@
       <c r="C97">
         <v>514</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -2002,8 +2296,11 @@
       <c r="C98">
         <v>514</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
@@ -2013,8 +2310,11 @@
       <c r="C99">
         <v>514</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
@@ -2024,8 +2324,11 @@
       <c r="C100">
         <v>514</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
@@ -2035,8 +2338,11 @@
       <c r="C101">
         <v>514</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
@@ -2046,8 +2352,11 @@
       <c r="C102">
         <v>514</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -2057,8 +2366,11 @@
       <c r="C103">
         <v>514</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
@@ -2068,8 +2380,11 @@
       <c r="C104">
         <v>514</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
@@ -2079,8 +2394,11 @@
       <c r="C105">
         <v>514</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
@@ -2090,8 +2408,11 @@
       <c r="C106">
         <v>514</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
@@ -2101,8 +2422,11 @@
       <c r="C107">
         <v>514</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
@@ -2112,8 +2436,11 @@
       <c r="C108">
         <v>514</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
@@ -2123,8 +2450,11 @@
       <c r="C109">
         <v>514</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
@@ -2134,8 +2464,11 @@
       <c r="C110">
         <v>514</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
@@ -2145,8 +2478,11 @@
       <c r="C111">
         <v>514</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -2156,8 +2492,11 @@
       <c r="C112">
         <v>514</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
@@ -2167,8 +2506,11 @@
       <c r="C113">
         <v>514</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
@@ -2178,8 +2520,11 @@
       <c r="C114">
         <v>514</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>118</v>
       </c>
@@ -2189,8 +2534,11 @@
       <c r="C115">
         <v>514</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>119</v>
       </c>
@@ -2200,8 +2548,11 @@
       <c r="C116">
         <v>514</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>120</v>
       </c>
@@ -2211,8 +2562,11 @@
       <c r="C117">
         <v>514</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>122</v>
       </c>
@@ -2222,8 +2576,11 @@
       <c r="C118">
         <v>588</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>121</v>
       </c>
@@ -2233,8 +2590,11 @@
       <c r="C119">
         <v>588</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>123</v>
       </c>
@@ -2244,8 +2604,11 @@
       <c r="C120">
         <v>588</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>124</v>
       </c>
@@ -2255,8 +2618,11 @@
       <c r="C121">
         <v>588</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>125</v>
       </c>
@@ -2266,8 +2632,11 @@
       <c r="C122">
         <v>588</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>126</v>
       </c>
@@ -2277,8 +2646,11 @@
       <c r="C123">
         <v>588</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>127</v>
       </c>
@@ -2288,8 +2660,11 @@
       <c r="C124">
         <v>588</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>128</v>
       </c>
@@ -2299,8 +2674,11 @@
       <c r="C125">
         <v>588</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
@@ -2310,8 +2688,11 @@
       <c r="C126">
         <v>588</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
@@ -2321,8 +2702,11 @@
       <c r="C127">
         <v>588</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
@@ -2332,8 +2716,11 @@
       <c r="C128">
         <v>588</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>132</v>
       </c>
@@ -2343,8 +2730,11 @@
       <c r="C129">
         <v>588</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>133</v>
       </c>
@@ -2354,8 +2744,11 @@
       <c r="C130">
         <v>588</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>134</v>
       </c>
@@ -2365,8 +2758,11 @@
       <c r="C131">
         <v>588</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>135</v>
       </c>
@@ -2376,8 +2772,11 @@
       <c r="C132">
         <v>588</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>136</v>
       </c>
@@ -2387,8 +2786,11 @@
       <c r="C133">
         <v>588</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>137</v>
       </c>
@@ -2398,8 +2800,11 @@
       <c r="C134">
         <v>588</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>138</v>
       </c>
@@ -2409,8 +2814,11 @@
       <c r="C135">
         <v>588</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>139</v>
       </c>
@@ -2420,8 +2828,11 @@
       <c r="C136">
         <v>588</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>140</v>
       </c>
@@ -2431,8 +2842,11 @@
       <c r="C137">
         <v>588</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>141</v>
       </c>
@@ -2442,8 +2856,11 @@
       <c r="C138">
         <v>588</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>142</v>
       </c>
@@ -2453,8 +2870,11 @@
       <c r="C139">
         <v>588</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>143</v>
       </c>
@@ -2464,8 +2884,11 @@
       <c r="C140">
         <v>588</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>144</v>
       </c>
@@ -2475,8 +2898,11 @@
       <c r="C141">
         <v>588</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>145</v>
       </c>
@@ -2486,8 +2912,11 @@
       <c r="C142">
         <v>588</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>146</v>
       </c>
@@ -2497,8 +2926,11 @@
       <c r="C143">
         <v>588</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>147</v>
       </c>
@@ -2508,8 +2940,11 @@
       <c r="C144">
         <v>588</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>148</v>
       </c>
@@ -2519,8 +2954,11 @@
       <c r="C145">
         <v>588</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -2530,8 +2968,11 @@
       <c r="C146">
         <v>588</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -2541,8 +2982,11 @@
       <c r="C147">
         <v>588</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>168</v>
       </c>
@@ -2552,8 +2996,11 @@
       <c r="C148">
         <v>588</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -2563,8 +3010,11 @@
       <c r="C149">
         <v>588</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>152</v>
       </c>
@@ -2574,8 +3024,11 @@
       <c r="C150">
         <v>588</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>153</v>
       </c>
@@ -2585,8 +3038,11 @@
       <c r="C151">
         <v>735</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>154</v>
       </c>
@@ -2596,8 +3052,11 @@
       <c r="C152">
         <v>735</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>155</v>
       </c>
@@ -2607,8 +3066,11 @@
       <c r="C153">
         <v>735</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>156</v>
       </c>
@@ -2618,8 +3080,11 @@
       <c r="C154">
         <v>735</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>157</v>
       </c>
@@ -2629,8 +3094,11 @@
       <c r="C155">
         <v>735</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>158</v>
       </c>
@@ -2640,8 +3108,11 @@
       <c r="C156">
         <v>735</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>159</v>
       </c>
@@ -2651,8 +3122,11 @@
       <c r="C157">
         <v>735</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>160</v>
       </c>
@@ -2662,8 +3136,11 @@
       <c r="C158">
         <v>845</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>161</v>
       </c>
@@ -2673,8 +3150,11 @@
       <c r="C159">
         <v>882</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>162</v>
       </c>
@@ -2684,8 +3164,11 @@
       <c r="C160">
         <v>882</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>163</v>
       </c>
@@ -2695,8 +3178,11 @@
       <c r="C161">
         <v>882</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>164</v>
       </c>
@@ -2706,8 +3192,11 @@
       <c r="C162">
         <v>992</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>165</v>
       </c>
@@ -2717,8 +3206,11 @@
       <c r="C163">
         <v>1102</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>166</v>
       </c>
@@ -2727,6 +3219,9 @@
       </c>
       <c r="C164">
         <v>1176</v>
+      </c>
+      <c r="D164">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>